<commit_message>
Modify design for 3d print output
</commit_message>
<xml_diff>
--- a/3d modeling/part list.xlsx
+++ b/3d modeling/part list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mokhw\Desktop\GitHub\gyroscope-drone\3d modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43466A81-C8C6-4C8E-8FFE-13776BE8956C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72DCB43-D988-4494-981F-86925B019148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F276262A-D9E6-428D-93CB-A151E407799A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
   <si>
     <t>axis</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -184,22 +184,6 @@
   </si>
   <si>
     <t>connector0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>connector1-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>connector1-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>connector2-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>connector2-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -248,18 +232,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>6hub-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6hub-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5hub-axis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>hemisphere</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -277,6 +249,19 @@
   </si>
   <si>
     <t>carbon fiber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sphere
+(d = 480)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gyro-drone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>340*40</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -299,14 +284,15 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">3*140.3 </t>
+      <t xml:space="preserve">3*140.33 </t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">inner </t>
-    </r>
+    <t>6hub-hemisphere</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -326,8 +312,11 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">380, outer </t>
+      <t>4*25</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -344,11 +333,48 @@
         <color theme="1"/>
         <rFont val="맑은 고딕"/>
         <family val="2"/>
-        <charset val="129"/>
+        <charset val="161"/>
         <scheme val="minor"/>
       </rPr>
-      <t>400</t>
+      <t>4*20</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6hub</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>connector1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>connector1_roll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>connector1_pitch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>connector2</t>
+  </si>
+  <si>
+    <t>connector2_pitch</t>
+  </si>
+  <si>
+    <t>connector2_yaw</t>
+  </si>
+  <si>
+    <t>no hole</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5hub-axis-bottom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5hub-axis-top</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -359,101 +385,30 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="161"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
       </rPr>
-      <t>Φ</t>
+      <t>Φ380, outer Φ400</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">inner </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>42</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
+        <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">0, outer </t>
+      <t>Φ420, outer Φ440</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="161"/>
-      </rPr>
-      <t>Φ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>44</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="161"/>
-      </rPr>
-      <t>Φ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">4*20 </t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sphere
-(d = 480)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gyro-drone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>340*40</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -464,7 +419,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,13 +486,6 @@
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
       <charset val="161"/>
       <scheme val="minor"/>
     </font>
@@ -573,7 +521,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -596,6 +544,194 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -614,7 +750,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -648,17 +784,113 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1167,10 +1399,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970BF917-3C4B-4060-9431-51718C7CB961}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1186,15 +1418,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
@@ -1205,22 +1437,22 @@
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
@@ -1230,361 +1462,440 @@
       <c r="C3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>43</v>
+      <c r="F3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="15">
+      <c r="A4" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="41">
         <v>1</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="21">
         <v>1</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7">
+      <c r="F4" s="22"/>
+      <c r="G4" s="23">
         <v>2</v>
       </c>
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="7">
+      <c r="A5" s="42"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="24">
         <v>2</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>28</v>
       </c>
       <c r="F5" s="7"/>
-      <c r="G5" s="7">
+      <c r="G5" s="25">
         <v>4</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="7">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="42"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="26">
         <v>3</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7">
+      <c r="F6" s="27"/>
+      <c r="G6" s="28">
         <v>1</v>
       </c>
       <c r="I6" s="9"/>
       <c r="L6" s="10"/>
     </row>
     <row r="7" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15">
+      <c r="A7" s="42"/>
+      <c r="B7" s="41">
         <v>2</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="13">
         <v>1</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="15">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="42"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="16">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="31">
+        <v>8</v>
+      </c>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="42"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="17">
+        <v>3</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="33">
+        <v>8</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="42"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="13">
+        <v>4</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="29"/>
+      <c r="G10" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="42"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="16">
+        <v>5</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="42"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="16">
+        <v>6</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="42"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="16">
+        <v>7</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="42"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="16">
+        <v>8</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="42"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="16">
+        <v>9</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="17">
+        <v>10</v>
+      </c>
+      <c r="E16" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="8">
+      <c r="F16" s="32"/>
+      <c r="G16" s="33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="13">
+        <v>11</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="16">
+        <v>12</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="42"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="17">
+        <v>13</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="42"/>
+      <c r="B20" s="41">
+        <v>3</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="13">
         <v>1</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="9">
+      <c r="E20" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="15">
+        <v>60</v>
+      </c>
+      <c r="H20">
+        <f>140.33*G20</f>
+        <v>8419.8000000000011</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="42"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="17">
         <v>2</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9">
+      <c r="E21" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="19">
+        <v>60</v>
+      </c>
+      <c r="H21">
+        <f>123.17*G21</f>
+        <v>7390.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="42"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="13">
+        <v>3</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="29"/>
+      <c r="G22" s="30">
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <f>SUM(H20:H21)</f>
+        <v>15810</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="42"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="16">
+        <v>4</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="31">
         <v>2</v>
       </c>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="8">
-        <v>3</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="8">
-        <v>1</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="9">
-        <v>4</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9">
+    </row>
+    <row r="24" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="42"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="16">
+        <v>5</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="37"/>
+      <c r="G24" s="31">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="9">
-        <v>5</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="8">
+    <row r="25" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="42"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="16">
         <v>6</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="9">
+      <c r="E25" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" s="9"/>
+      <c r="G25" s="31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="17">
         <v>7</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="9">
-        <v>8</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="7">
-        <v>9</v>
-      </c>
-      <c r="E15" s="7" t="s">
+      <c r="E26" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="7">
+      <c r="G26" s="33">
         <v>10</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15">
-        <v>3</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="8">
-        <v>1</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" s="8">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="8">
-        <v>2</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" s="8">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="9">
-        <v>3</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="9">
-        <v>4</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G20" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="9">
-        <v>5</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="9">
-        <v>6</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="9">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="C20:C26"/>
+    <mergeCell ref="B20:B26"/>
+    <mergeCell ref="A4:A26"/>
+    <mergeCell ref="B7:B19"/>
+    <mergeCell ref="C7:C19"/>
+    <mergeCell ref="C4:C6"/>
     <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="B17:B22"/>
-    <mergeCell ref="A4:A22"/>
-    <mergeCell ref="B7:B16"/>
-    <mergeCell ref="C7:C16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modify 3d print design 3
</commit_message>
<xml_diff>
--- a/3d modeling/part list.xlsx
+++ b/3d modeling/part list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mokhw\Desktop\GitHub\gyroscope-drone\3d modeling\gyro-drone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mokhw\Desktop\GitHub\gyroscope-drone\3d modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FF4019-222B-40BE-B569-7D87BE3E82D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13844634-FBD4-43A0-AD80-FBA2A30CEA76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F276262A-D9E6-428D-93CB-A151E407799A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
   <si>
     <t>axis</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -340,6 +340,10 @@
   </si>
   <si>
     <t>sindoh(신도리코) DP102(DP200)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무게 1kg 이내로</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -944,6 +948,24 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -990,24 +1012,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1518,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970BF917-3C4B-4060-9431-51718C7CB961}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1535,16 +1539,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="4"/>
@@ -1555,17 +1559,17 @@
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46" t="s">
+      <c r="C2" s="52"/>
+      <c r="D2" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
       <c r="I2" s="8"/>
       <c r="J2" s="6"/>
       <c r="K2" s="4"/>
@@ -1601,13 +1605,13 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="52">
+      <c r="B4" s="58">
         <v>1</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="61" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="11">
@@ -1617,7 +1621,7 @@
         <v>27</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="58">
+      <c r="G4" s="64">
         <v>468</v>
       </c>
       <c r="H4" s="13">
@@ -1627,9 +1631,9 @@
       <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="56"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="62"/>
       <c r="D5" s="15">
         <v>2</v>
       </c>
@@ -1637,7 +1641,7 @@
         <v>28</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="59"/>
+      <c r="G5" s="65"/>
       <c r="H5" s="16">
         <v>4</v>
       </c>
@@ -1647,9 +1651,9 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="57"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="63"/>
       <c r="D6" s="17">
         <v>3</v>
       </c>
@@ -1657,20 +1661,22 @@
         <v>29</v>
       </c>
       <c r="F6" s="18"/>
-      <c r="G6" s="60"/>
+      <c r="G6" s="66"/>
       <c r="H6" s="19">
         <v>1</v>
       </c>
-      <c r="I6" s="8"/>
+      <c r="I6" s="8">
+        <v>468</v>
+      </c>
       <c r="J6" s="20"/>
       <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="53"/>
-      <c r="B7" s="52">
+      <c r="A7" s="59"/>
+      <c r="B7" s="58">
         <v>2</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="61" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="21">
@@ -1688,15 +1694,18 @@
       <c r="H7" s="23">
         <v>1</v>
       </c>
-      <c r="I7" s="8"/>
+      <c r="I7" s="8">
+        <f>SUM(G7*H7)</f>
+        <v>36</v>
+      </c>
       <c r="J7" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="53"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="56"/>
+      <c r="A8" s="59"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="62"/>
       <c r="D8" s="24">
         <v>2</v>
       </c>
@@ -1706,17 +1715,22 @@
       <c r="F8" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="G8" s="38"/>
+      <c r="G8" s="38">
+        <v>10</v>
+      </c>
       <c r="H8" s="25">
         <v>8</v>
       </c>
-      <c r="I8" s="8"/>
+      <c r="I8" s="8">
+        <f t="shared" ref="I8:I16" si="0">SUM(G8*H8)</f>
+        <v>80</v>
+      </c>
       <c r="J8" s="26"/>
     </row>
     <row r="9" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="53"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="56"/>
+      <c r="A9" s="59"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="62"/>
       <c r="D9" s="27">
         <v>3</v>
       </c>
@@ -1730,15 +1744,18 @@
       <c r="H9" s="29">
         <v>8</v>
       </c>
-      <c r="I9" s="8"/>
+      <c r="I9" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="J9" s="7" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="53"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="56"/>
+      <c r="A10" s="59"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="62"/>
       <c r="D10" s="21">
         <v>4</v>
       </c>
@@ -1746,17 +1763,22 @@
         <v>37</v>
       </c>
       <c r="F10" s="30"/>
-      <c r="G10" s="40"/>
+      <c r="G10" s="40">
+        <v>12</v>
+      </c>
       <c r="H10" s="31">
         <v>4</v>
       </c>
-      <c r="I10" s="8"/>
+      <c r="I10" s="8">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="53"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="56"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="62"/>
       <c r="D11" s="24">
         <v>5</v>
       </c>
@@ -1766,21 +1788,26 @@
       <c r="F11" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="38"/>
+      <c r="G11" s="38">
+        <v>4</v>
+      </c>
       <c r="H11" s="25">
         <v>8</v>
       </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="64" t="s">
+      <c r="I11" s="8">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="J11" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="K11" s="65"/>
-      <c r="L11" s="66"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="47"/>
     </row>
     <row r="12" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="53"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="56"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="62"/>
       <c r="D12" s="24">
         <v>6</v>
       </c>
@@ -1788,21 +1815,26 @@
         <v>57</v>
       </c>
       <c r="F12" s="20"/>
-      <c r="G12" s="38"/>
+      <c r="G12" s="38">
+        <v>4</v>
+      </c>
       <c r="H12" s="25">
         <v>4</v>
       </c>
-      <c r="I12" s="8"/>
-      <c r="J12" s="61" t="s">
+      <c r="I12" s="8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="J12" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="K12" s="62"/>
-      <c r="L12" s="63"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="50"/>
     </row>
     <row r="13" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="53"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="56"/>
+      <c r="A13" s="59"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="62"/>
       <c r="D13" s="24">
         <v>7</v>
       </c>
@@ -1810,17 +1842,22 @@
         <v>58</v>
       </c>
       <c r="F13" s="20"/>
-      <c r="G13" s="38"/>
+      <c r="G13" s="38">
+        <v>4</v>
+      </c>
       <c r="H13" s="25">
         <v>4</v>
       </c>
-      <c r="I13" s="8"/>
+      <c r="I13" s="8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="53"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="56"/>
+      <c r="A14" s="59"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="62"/>
       <c r="D14" s="24">
         <v>8</v>
       </c>
@@ -1834,13 +1871,16 @@
       <c r="H14" s="25">
         <v>8</v>
       </c>
-      <c r="I14" s="8"/>
+      <c r="I14" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="53"/>
-      <c r="B15" s="53"/>
-      <c r="C15" s="56"/>
+      <c r="A15" s="59"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="62"/>
       <c r="D15" s="24">
         <v>9</v>
       </c>
@@ -1852,13 +1892,20 @@
       <c r="H15" s="25">
         <v>4</v>
       </c>
-      <c r="I15" s="8"/>
+      <c r="I15" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="J15" s="8"/>
+      <c r="L15">
+        <f>56*2</f>
+        <v>112</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="53"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="56"/>
+      <c r="A16" s="59"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="62"/>
       <c r="D16" s="27">
         <v>10</v>
       </c>
@@ -1870,13 +1917,16 @@
       <c r="H16" s="29">
         <v>4</v>
       </c>
-      <c r="I16" s="8"/>
+      <c r="I16" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="53"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="56"/>
+      <c r="A17" s="59"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="62"/>
       <c r="D17" s="24">
         <v>11</v>
       </c>
@@ -1892,13 +1942,15 @@
       <c r="H17" s="16">
         <v>6</v>
       </c>
-      <c r="I17" s="8"/>
+      <c r="I17" s="8">
+        <v>12</v>
+      </c>
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="53"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="57"/>
+      <c r="A18" s="59"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="63"/>
       <c r="D18" s="27">
         <v>12</v>
       </c>
@@ -1918,11 +1970,11 @@
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="53"/>
-      <c r="B19" s="52">
+      <c r="A19" s="59"/>
+      <c r="B19" s="58">
         <v>3</v>
       </c>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="55" t="s">
         <v>51</v>
       </c>
       <c r="D19" s="21">
@@ -1941,15 +1993,14 @@
         <v>60</v>
       </c>
       <c r="I19" s="8">
-        <f>140.33*H19</f>
-        <v>8419.8000000000011</v>
+        <v>91</v>
       </c>
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="53"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="50"/>
+      <c r="A20" s="59"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="56"/>
       <c r="D20" s="27">
         <v>2</v>
       </c>
@@ -1966,15 +2017,14 @@
         <v>60</v>
       </c>
       <c r="I20" s="8">
-        <f>123.17*H20</f>
-        <v>7390.2</v>
+        <v>80</v>
       </c>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="53"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="50"/>
+      <c r="A21" s="59"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="56"/>
       <c r="D21" s="21">
         <v>3</v>
       </c>
@@ -1986,23 +2036,20 @@
       <c r="H21" s="31">
         <v>10</v>
       </c>
-      <c r="I21" s="8">
-        <f>SUM(I19:I20)</f>
-        <v>15810</v>
-      </c>
+      <c r="I21" s="8"/>
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="53"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="50"/>
+      <c r="A22" s="59"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="56"/>
       <c r="D22" s="24">
         <v>4</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="47" t="s">
+      <c r="F22" s="53" t="s">
         <v>47</v>
       </c>
       <c r="G22" s="43"/>
@@ -2013,16 +2060,16 @@
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="53"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="50"/>
+      <c r="A23" s="59"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="56"/>
       <c r="D23" s="24">
         <v>5</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="F23" s="48"/>
+      <c r="F23" s="54"/>
       <c r="G23" s="44"/>
       <c r="H23" s="25">
         <v>2</v>
@@ -2031,9 +2078,9 @@
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="53"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="50"/>
+      <c r="A24" s="59"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="56"/>
       <c r="D24" s="24">
         <v>6</v>
       </c>
@@ -2049,9 +2096,9 @@
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="54"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="51"/>
+      <c r="A25" s="60"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="57"/>
       <c r="D25" s="27">
         <v>7</v>
       </c>
@@ -2069,18 +2116,16 @@
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G26">
-        <f>SUM(G4:G25)</f>
-        <v>687</v>
+      <c r="I26">
+        <f>SUM(I4:I25)</f>
+        <v>879</v>
+      </c>
+      <c r="J26" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="B2:C2"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="C19:C25"/>
     <mergeCell ref="B19:B25"/>
@@ -2089,6 +2134,11 @@
     <mergeCell ref="C7:C18"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="B4:B6"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="B2:C2"/>
     <mergeCell ref="G4:G6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Modify 3d print design 4
</commit_message>
<xml_diff>
--- a/3d modeling/part list.xlsx
+++ b/3d modeling/part list.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mokhw\Desktop\GitHub\gyroscope-drone\3d modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13844634-FBD4-43A0-AD80-FBA2A30CEA76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12846AC-8DA7-422C-9829-2D1D9AC5F651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F276262A-D9E6-428D-93CB-A151E407799A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F276262A-D9E6-428D-93CB-A151E407799A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="2021-03-31" sheetId="2" r:id="rId2"/>
+    <sheet name="2021-04-01" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="94">
   <si>
     <t>axis</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -346,6 +347,145 @@
     <t>무게 1kg 이내로</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>frame</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Φ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">3*140.33 </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bracket</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yaw bracket</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pitch bracket</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>size (mm)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3d print</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">inner </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Φ420, outer Φ440, thickness 10</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">inner </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Φ380, outer Φ400, thickness 10</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">inner </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Φ4, outer Φ7, width 2.5</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>roll-ring</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pitch-ring</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yaw-sphere</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[roll-ring] frame</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[roll-ring] bracket-basic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[roll-ring] bracket-roll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[roll-ring] bracket-pitch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[mount] frame</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[mount] bracket</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -354,7 +494,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,6 +570,14 @@
       <family val="3"/>
       <charset val="161"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -473,7 +621,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -788,6 +936,212 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -812,7 +1166,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -948,27 +1302,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1005,6 +1338,30 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1013,6 +1370,126 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1522,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970BF917-3C4B-4060-9431-51718C7CB961}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1539,16 +2016,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="4"/>
@@ -1559,17 +2036,17 @@
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52" t="s">
+      <c r="C2" s="64"/>
+      <c r="D2" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
       <c r="I2" s="8"/>
       <c r="J2" s="6"/>
       <c r="K2" s="4"/>
@@ -1605,13 +2082,13 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="58">
+      <c r="B4" s="51">
         <v>1</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="54" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="11">
@@ -1621,7 +2098,7 @@
         <v>27</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="64">
+      <c r="G4" s="65">
         <v>468</v>
       </c>
       <c r="H4" s="13">
@@ -1631,9 +2108,9 @@
       <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="59"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="62"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="55"/>
       <c r="D5" s="15">
         <v>2</v>
       </c>
@@ -1641,7 +2118,7 @@
         <v>28</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="65"/>
+      <c r="G5" s="66"/>
       <c r="H5" s="16">
         <v>4</v>
       </c>
@@ -1651,9 +2128,9 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="59"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="63"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="17">
         <v>3</v>
       </c>
@@ -1661,7 +2138,7 @@
         <v>29</v>
       </c>
       <c r="F6" s="18"/>
-      <c r="G6" s="66"/>
+      <c r="G6" s="67"/>
       <c r="H6" s="19">
         <v>1</v>
       </c>
@@ -1672,11 +2149,11 @@
       <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="59"/>
-      <c r="B7" s="58">
+      <c r="A7" s="52"/>
+      <c r="B7" s="51">
         <v>2</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="54" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="21">
@@ -1703,9 +2180,9 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="59"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="62"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="55"/>
       <c r="D8" s="24">
         <v>2</v>
       </c>
@@ -1728,9 +2205,9 @@
       <c r="J8" s="26"/>
     </row>
     <row r="9" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="59"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="62"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="55"/>
       <c r="D9" s="27">
         <v>3</v>
       </c>
@@ -1753,9 +2230,9 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="59"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="62"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="55"/>
       <c r="D10" s="21">
         <v>4</v>
       </c>
@@ -1776,9 +2253,9 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="59"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="62"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="55"/>
       <c r="D11" s="24">
         <v>5</v>
       </c>
@@ -1798,16 +2275,16 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="J11" s="45" t="s">
+      <c r="J11" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="K11" s="46"/>
-      <c r="L11" s="47"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="59"/>
     </row>
     <row r="12" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="59"/>
-      <c r="B12" s="59"/>
-      <c r="C12" s="62"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="55"/>
       <c r="D12" s="24">
         <v>6</v>
       </c>
@@ -1825,16 +2302,16 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="J12" s="48" t="s">
+      <c r="J12" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="K12" s="49"/>
-      <c r="L12" s="50"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="62"/>
     </row>
     <row r="13" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="59"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="62"/>
+      <c r="A13" s="52"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="55"/>
       <c r="D13" s="24">
         <v>7</v>
       </c>
@@ -1855,9 +2332,9 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="59"/>
-      <c r="B14" s="59"/>
-      <c r="C14" s="62"/>
+      <c r="A14" s="52"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="55"/>
       <c r="D14" s="24">
         <v>8</v>
       </c>
@@ -1878,9 +2355,9 @@
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="59"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="62"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="55"/>
       <c r="D15" s="24">
         <v>9</v>
       </c>
@@ -1903,9 +2380,9 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="59"/>
-      <c r="B16" s="59"/>
-      <c r="C16" s="62"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="55"/>
       <c r="D16" s="27">
         <v>10</v>
       </c>
@@ -1924,9 +2401,9 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="59"/>
-      <c r="B17" s="59"/>
-      <c r="C17" s="62"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="55"/>
       <c r="D17" s="24">
         <v>11</v>
       </c>
@@ -1948,9 +2425,9 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="59"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="63"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="56"/>
       <c r="D18" s="27">
         <v>12</v>
       </c>
@@ -1970,11 +2447,11 @@
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="59"/>
-      <c r="B19" s="58">
+      <c r="A19" s="52"/>
+      <c r="B19" s="51">
         <v>3</v>
       </c>
-      <c r="C19" s="55" t="s">
+      <c r="C19" s="48" t="s">
         <v>51</v>
       </c>
       <c r="D19" s="21">
@@ -1998,9 +2475,9 @@
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="59"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="56"/>
+      <c r="A20" s="52"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="27">
         <v>2</v>
       </c>
@@ -2022,9 +2499,9 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="59"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="56"/>
+      <c r="A21" s="52"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="49"/>
       <c r="D21" s="21">
         <v>3</v>
       </c>
@@ -2040,16 +2517,16 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="59"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="56"/>
+      <c r="A22" s="52"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="49"/>
       <c r="D22" s="24">
         <v>4</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="53" t="s">
+      <c r="F22" s="46" t="s">
         <v>47</v>
       </c>
       <c r="G22" s="43"/>
@@ -2060,16 +2537,16 @@
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="59"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="56"/>
+      <c r="A23" s="52"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="24">
         <v>5</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="F23" s="54"/>
+      <c r="F23" s="47"/>
       <c r="G23" s="44"/>
       <c r="H23" s="25">
         <v>2</v>
@@ -2078,9 +2555,9 @@
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="59"/>
-      <c r="B24" s="59"/>
-      <c r="C24" s="56"/>
+      <c r="A24" s="52"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="49"/>
       <c r="D24" s="24">
         <v>6</v>
       </c>
@@ -2096,9 +2573,9 @@
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="60"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="57"/>
+      <c r="A25" s="53"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="27">
         <v>7</v>
       </c>
@@ -2126,6 +2603,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G4:G6"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="C19:C25"/>
     <mergeCell ref="B19:B25"/>
@@ -2134,12 +2617,635 @@
     <mergeCell ref="C7:C18"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="B4:B6"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="G4:G6"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49756507-D464-4B18-B1BA-D41ABE0D1473}">
+  <dimension ref="A1:M28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
+    <col min="2" max="2" width="10.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="40.5" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="8" max="8" width="8.5" customWidth="1"/>
+    <col min="10" max="10" width="16.75" customWidth="1"/>
+    <col min="11" max="11" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="95" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="90" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="95" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="87" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="86" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="87" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="87" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="87" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="96" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="92">
+        <v>1</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="78">
+        <v>1</v>
+      </c>
+      <c r="E3" s="100" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="71"/>
+      <c r="G3" s="68">
+        <v>468</v>
+      </c>
+      <c r="H3" s="71">
+        <v>2</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="14"/>
+    </row>
+    <row r="4" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="69"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="79">
+        <v>2</v>
+      </c>
+      <c r="E4" s="101" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="72"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="72">
+        <v>4</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="69"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="80">
+        <v>3</v>
+      </c>
+      <c r="E5" s="102" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="73"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="73">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="L5" s="58"/>
+      <c r="M5" s="59"/>
+    </row>
+    <row r="6" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="69"/>
+      <c r="B6" s="92">
+        <v>2</v>
+      </c>
+      <c r="C6" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="97">
+        <v>1</v>
+      </c>
+      <c r="E6" s="103" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="98" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="98">
+        <v>36</v>
+      </c>
+      <c r="H6" s="98">
+        <v>1</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="L6" s="61"/>
+      <c r="M6" s="62"/>
+    </row>
+    <row r="7" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="69"/>
+      <c r="B7" s="93"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="81">
+        <v>2</v>
+      </c>
+      <c r="E7" s="104" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74">
+        <v>4</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="26"/>
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="1:13" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="69"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="82">
+        <v>3</v>
+      </c>
+      <c r="E8" s="105" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="75" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75">
+        <v>4</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="69"/>
+      <c r="B9" s="92">
+        <v>3</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="83">
+        <v>1</v>
+      </c>
+      <c r="E9" s="106" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="76">
+        <v>10</v>
+      </c>
+      <c r="H9" s="76">
+        <v>8</v>
+      </c>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="69"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="81">
+        <v>2</v>
+      </c>
+      <c r="E10" s="104" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74">
+        <v>8</v>
+      </c>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="69"/>
+      <c r="B11" s="93"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="81">
+        <v>3</v>
+      </c>
+      <c r="E11" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74">
+        <v>4</v>
+      </c>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="69"/>
+      <c r="B12" s="93"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="81">
+        <v>4</v>
+      </c>
+      <c r="E12" s="104" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74">
+        <v>12</v>
+      </c>
+      <c r="H12" s="74">
+        <v>4</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="69"/>
+      <c r="B13" s="93"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="84">
+        <v>5</v>
+      </c>
+      <c r="E13" s="107" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="77">
+        <v>12</v>
+      </c>
+      <c r="H13" s="77">
+        <v>2</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="69"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="82">
+        <v>6</v>
+      </c>
+      <c r="E14" s="105" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="75" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="75">
+        <v>0</v>
+      </c>
+      <c r="H14" s="75">
+        <v>8</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="69"/>
+      <c r="B15" s="92">
+        <v>4</v>
+      </c>
+      <c r="C15" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="83">
+        <v>1</v>
+      </c>
+      <c r="E15" s="106" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="76" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76">
+        <v>8</v>
+      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="69"/>
+      <c r="B16" s="93"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="81">
+        <v>2</v>
+      </c>
+      <c r="E16" s="104" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="74">
+        <v>8</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="69"/>
+      <c r="B17" s="93"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="81">
+        <v>3</v>
+      </c>
+      <c r="E17" s="104" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74">
+        <v>4</v>
+      </c>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="69"/>
+      <c r="B18" s="93"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="81">
+        <v>4</v>
+      </c>
+      <c r="E18" s="104" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="74"/>
+      <c r="G18" s="74"/>
+      <c r="H18" s="74">
+        <v>4</v>
+      </c>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="69"/>
+      <c r="B19" s="93"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="84">
+        <v>5</v>
+      </c>
+      <c r="E19" s="107" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="77"/>
+      <c r="H19" s="77">
+        <v>2</v>
+      </c>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="69"/>
+      <c r="B20" s="94"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="82">
+        <v>6</v>
+      </c>
+      <c r="E20" s="105" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="75" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="75"/>
+      <c r="H20" s="75">
+        <v>8</v>
+      </c>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="69"/>
+      <c r="B21" s="92">
+        <v>5</v>
+      </c>
+      <c r="C21" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="78">
+        <v>1</v>
+      </c>
+      <c r="E21" s="100" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="71" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="71">
+        <v>91</v>
+      </c>
+      <c r="H21" s="71">
+        <v>60</v>
+      </c>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="69"/>
+      <c r="B22" s="93"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="79">
+        <v>2</v>
+      </c>
+      <c r="E22" s="101" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="72">
+        <v>80</v>
+      </c>
+      <c r="H22" s="72">
+        <v>60</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="69"/>
+      <c r="B23" s="93"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="79">
+        <v>3</v>
+      </c>
+      <c r="E23" s="101" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="72"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="72">
+        <v>10</v>
+      </c>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="69"/>
+      <c r="B24" s="93"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="79">
+        <v>4</v>
+      </c>
+      <c r="E24" s="101" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="72"/>
+      <c r="H24" s="72">
+        <v>2</v>
+      </c>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="69"/>
+      <c r="B25" s="93"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="79">
+        <v>5</v>
+      </c>
+      <c r="E25" s="101" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="69"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="72">
+        <v>2</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="69"/>
+      <c r="B26" s="93"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="80">
+        <v>6</v>
+      </c>
+      <c r="E26" s="101" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" s="72"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="72">
+        <v>20</v>
+      </c>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="70"/>
+      <c r="B27" s="94"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="85">
+        <v>7</v>
+      </c>
+      <c r="E27" s="102" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="73"/>
+      <c r="H27" s="73">
+        <v>10</v>
+      </c>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B21:B27"/>
+    <mergeCell ref="C21:C27"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="A3:A27"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="G3:G5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modify 3d print design 5
</commit_message>
<xml_diff>
--- a/3d modeling/part list.xlsx
+++ b/3d modeling/part list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mokhw\Desktop\GitHub\gyroscope-drone\3d modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12846AC-8DA7-422C-9829-2D1D9AC5F651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4CC53F-3B73-4735-BB62-EE99FC6253C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F276262A-D9E6-428D-93CB-A151E407799A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="98">
   <si>
     <t>axis</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -348,7 +348,67 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>frame</t>
+    <t>mount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>size (mm)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3d print</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>roll-ring</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pitch-ring</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[roll-ring] frame</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[roll-ring] bracket-basic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[roll-ring] bracket-roll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[roll-ring] bracket-pitch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[mount] frame</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[mount] bracket</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inner Φ4, outer Φ7, width 2.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inner Φ380, outer Φ400, thickness 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inner Φ420, outer Φ440, thickness 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Φ3*140 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Φ3*123</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -366,125 +426,62 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="나눔고딕"/>
         <family val="3"/>
         <charset val="129"/>
-        <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">3*140.33 </t>
+      <t>4*25</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>bracket</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yaw bracket</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pitch bracket</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>size (mm)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3d print</t>
+    <t>[pitch-ring] frame</t>
+  </si>
+  <si>
+    <t>[pitch-ring] bracket-basic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[pitch-ring]  bracket-pitch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[pitch-ring]  bracket-yaw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yaw-sphere
+(d = 480mm)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">inner </t>
+      <t xml:space="preserve">hole </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
+        <charset val="161"/>
       </rPr>
-      <t>Φ420, outer Φ440, thickness 10</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">inner </t>
+      <t>Φ</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="나눔고딕"/>
         <family val="3"/>
         <charset val="129"/>
-        <scheme val="minor"/>
       </rPr>
-      <t>Φ380, outer Φ400, thickness 10</t>
+      <t>3.2</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">inner </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Φ4, outer Φ7, width 2.5</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>roll-ring</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pitch-ring</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yaw-sphere</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[roll-ring] frame</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[roll-ring] bracket-basic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[roll-ring] bracket-roll</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[roll-ring] bracket-pitch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[mount] frame</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[mount] bracket</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>hole Φ3.2</t>
   </si>
 </sst>
 </file>
@@ -494,7 +491,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -570,14 +567,6 @@
       <family val="3"/>
       <charset val="161"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1166,7 +1155,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1305,6 +1294,39 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1338,158 +1360,128 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="26" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="25" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2016,16 +2008,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="4"/>
@@ -2036,17 +2028,17 @@
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
       <c r="I2" s="8"/>
       <c r="J2" s="6"/>
       <c r="K2" s="4"/>
@@ -2082,13 +2074,13 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="51">
+      <c r="B4" s="62">
         <v>1</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="65" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="11">
@@ -2098,7 +2090,7 @@
         <v>27</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="65">
+      <c r="G4" s="54">
         <v>468</v>
       </c>
       <c r="H4" s="13">
@@ -2108,9 +2100,9 @@
       <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="55"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="66"/>
       <c r="D5" s="15">
         <v>2</v>
       </c>
@@ -2118,7 +2110,7 @@
         <v>28</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="66"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="16">
         <v>4</v>
       </c>
@@ -2128,9 +2120,9 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="52"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="56"/>
+      <c r="A6" s="63"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="67"/>
       <c r="D6" s="17">
         <v>3</v>
       </c>
@@ -2138,7 +2130,7 @@
         <v>29</v>
       </c>
       <c r="F6" s="18"/>
-      <c r="G6" s="67"/>
+      <c r="G6" s="56"/>
       <c r="H6" s="19">
         <v>1</v>
       </c>
@@ -2149,11 +2141,11 @@
       <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
-      <c r="B7" s="51">
+      <c r="A7" s="63"/>
+      <c r="B7" s="62">
         <v>2</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="65" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="21">
@@ -2180,9 +2172,9 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="55"/>
+      <c r="A8" s="63"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="66"/>
       <c r="D8" s="24">
         <v>2</v>
       </c>
@@ -2205,9 +2197,9 @@
       <c r="J8" s="26"/>
     </row>
     <row r="9" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="52"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="55"/>
+      <c r="A9" s="63"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="66"/>
       <c r="D9" s="27">
         <v>3</v>
       </c>
@@ -2230,9 +2222,9 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="55"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="21">
         <v>4</v>
       </c>
@@ -2253,9 +2245,9 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="55"/>
+      <c r="A11" s="63"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="24">
         <v>5</v>
       </c>
@@ -2275,16 +2267,16 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="J11" s="57" t="s">
+      <c r="J11" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="K11" s="58"/>
-      <c r="L11" s="59"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="48"/>
     </row>
     <row r="12" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="52"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="55"/>
+      <c r="A12" s="63"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="66"/>
       <c r="D12" s="24">
         <v>6</v>
       </c>
@@ -2302,16 +2294,16 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="J12" s="60" t="s">
+      <c r="J12" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="K12" s="61"/>
-      <c r="L12" s="62"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="51"/>
     </row>
     <row r="13" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="52"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="55"/>
+      <c r="A13" s="63"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="24">
         <v>7</v>
       </c>
@@ -2332,9 +2324,9 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="52"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="55"/>
+      <c r="A14" s="63"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="66"/>
       <c r="D14" s="24">
         <v>8</v>
       </c>
@@ -2355,9 +2347,9 @@
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="52"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="55"/>
+      <c r="A15" s="63"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="66"/>
       <c r="D15" s="24">
         <v>9</v>
       </c>
@@ -2380,9 +2372,9 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="55"/>
+      <c r="A16" s="63"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="66"/>
       <c r="D16" s="27">
         <v>10</v>
       </c>
@@ -2401,9 +2393,9 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="52"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="55"/>
+      <c r="A17" s="63"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="66"/>
       <c r="D17" s="24">
         <v>11</v>
       </c>
@@ -2425,9 +2417,9 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="52"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="56"/>
+      <c r="A18" s="63"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="67"/>
       <c r="D18" s="27">
         <v>12</v>
       </c>
@@ -2447,11 +2439,11 @@
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="52"/>
-      <c r="B19" s="51">
+      <c r="A19" s="63"/>
+      <c r="B19" s="62">
         <v>3</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="59" t="s">
         <v>51</v>
       </c>
       <c r="D19" s="21">
@@ -2475,9 +2467,9 @@
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="52"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="49"/>
+      <c r="A20" s="63"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="60"/>
       <c r="D20" s="27">
         <v>2</v>
       </c>
@@ -2499,9 +2491,9 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="52"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="49"/>
+      <c r="A21" s="63"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="60"/>
       <c r="D21" s="21">
         <v>3</v>
       </c>
@@ -2517,16 +2509,16 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="52"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="49"/>
+      <c r="A22" s="63"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="60"/>
       <c r="D22" s="24">
         <v>4</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="46" t="s">
+      <c r="F22" s="57" t="s">
         <v>47</v>
       </c>
       <c r="G22" s="43"/>
@@ -2537,16 +2529,16 @@
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="52"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="49"/>
+      <c r="A23" s="63"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="60"/>
       <c r="D23" s="24">
         <v>5</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="F23" s="47"/>
+      <c r="F23" s="58"/>
       <c r="G23" s="44"/>
       <c r="H23" s="25">
         <v>2</v>
@@ -2555,9 +2547,9 @@
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="52"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="49"/>
+      <c r="A24" s="63"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="60"/>
       <c r="D24" s="24">
         <v>6</v>
       </c>
@@ -2573,9 +2565,9 @@
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="53"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="50"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="61"/>
       <c r="D25" s="27">
         <v>7</v>
       </c>
@@ -2603,12 +2595,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="G4:G6"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="C19:C25"/>
     <mergeCell ref="B19:B25"/>
@@ -2617,6 +2603,12 @@
     <mergeCell ref="C7:C18"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="B4:B6"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G4:G6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2629,7 +2621,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2647,20 +2639,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88" t="s">
+      <c r="C1" s="70"/>
+      <c r="D1" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="89"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="71"/>
       <c r="I1" s="8"/>
       <c r="J1" s="6"/>
       <c r="K1" s="4"/>
@@ -2668,72 +2660,72 @@
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="99" t="s">
+      <c r="E2" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="87" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" s="87" t="s">
+      <c r="F2" s="73" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="87" t="s">
+      <c r="H2" s="73" t="s">
         <v>39</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="92">
+      <c r="B3" s="77">
         <v>1</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="78">
+      <c r="D3" s="79">
         <v>1</v>
       </c>
-      <c r="E3" s="100" t="s">
+      <c r="E3" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="71"/>
-      <c r="G3" s="68">
+      <c r="F3" s="81"/>
+      <c r="G3" s="78">
         <v>468</v>
       </c>
-      <c r="H3" s="71">
+      <c r="H3" s="81">
         <v>2</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69"/>
-      <c r="B4" s="93"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="79">
+      <c r="A4" s="82"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="83">
         <v>2</v>
       </c>
-      <c r="E4" s="101" t="s">
+      <c r="E4" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="72"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="72">
+      <c r="F4" s="85"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="85">
         <v>4</v>
       </c>
       <c r="I4" s="8"/>
@@ -2742,74 +2734,74 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="69"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="80">
+      <c r="A5" s="82"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="88">
         <v>3</v>
       </c>
-      <c r="E5" s="102" t="s">
+      <c r="E5" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="73"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="73">
+      <c r="F5" s="90"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="90">
         <v>1</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="58" t="s">
+      <c r="K5" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="L5" s="58"/>
-      <c r="M5" s="59"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="48"/>
     </row>
     <row r="6" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="69"/>
-      <c r="B6" s="92">
+      <c r="A6" s="82"/>
+      <c r="B6" s="77">
         <v>2</v>
       </c>
-      <c r="C6" s="68" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="97">
+      <c r="C6" s="78" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="91">
         <v>1</v>
       </c>
-      <c r="E6" s="103" t="s">
-        <v>92</v>
-      </c>
-      <c r="F6" s="98" t="s">
+      <c r="E6" s="92" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="98">
+      <c r="G6" s="93">
         <v>36</v>
       </c>
-      <c r="H6" s="98">
+      <c r="H6" s="93">
         <v>1</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="K6" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="K6" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="L6" s="61"/>
-      <c r="M6" s="62"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="51"/>
     </row>
     <row r="7" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="69"/>
-      <c r="B7" s="93"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="81">
+      <c r="A7" s="82"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="94">
         <v>2</v>
       </c>
-      <c r="E7" s="104" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74">
+      <c r="E7" s="95" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="96">
         <v>4</v>
       </c>
       <c r="I7" s="8"/>
@@ -2817,20 +2809,20 @@
       <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="69"/>
-      <c r="B8" s="94"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="82">
+      <c r="A8" s="82"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="97">
         <v>3</v>
       </c>
-      <c r="E8" s="105" t="s">
+      <c r="E8" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="75" t="s">
-        <v>84</v>
-      </c>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75">
+      <c r="F8" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="99"/>
+      <c r="H8" s="99">
         <v>4</v>
       </c>
       <c r="I8" s="8"/>
@@ -2840,383 +2832,389 @@
       <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="69"/>
-      <c r="B9" s="92">
+      <c r="A9" s="82"/>
+      <c r="B9" s="77">
         <v>3</v>
       </c>
-      <c r="C9" s="68" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="83">
+      <c r="C9" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="100">
         <v>1</v>
       </c>
-      <c r="E9" s="106" t="s">
-        <v>88</v>
-      </c>
-      <c r="F9" s="76" t="s">
-        <v>83</v>
-      </c>
-      <c r="G9" s="76">
+      <c r="E9" s="101" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="102" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="102">
         <v>10</v>
       </c>
-      <c r="H9" s="76">
+      <c r="H9" s="102">
         <v>8</v>
       </c>
       <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="69"/>
-      <c r="B10" s="93"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="81">
+      <c r="A10" s="82"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="94">
         <v>2</v>
       </c>
-      <c r="E10" s="104" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74">
+      <c r="E10" s="95" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96">
         <v>8</v>
       </c>
       <c r="I10" s="8"/>
     </row>
     <row r="11" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="69"/>
-      <c r="B11" s="93"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="81">
+      <c r="A11" s="82"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="94">
         <v>3</v>
       </c>
-      <c r="E11" s="104" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74">
+      <c r="E11" s="95" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="96">
         <v>4</v>
       </c>
       <c r="I11" s="8"/>
     </row>
     <row r="12" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="69"/>
-      <c r="B12" s="93"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="81">
+      <c r="A12" s="82"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="94">
         <v>4</v>
       </c>
-      <c r="E12" s="104" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74">
+      <c r="E12" s="95" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="96"/>
+      <c r="G12" s="96">
         <v>12</v>
       </c>
-      <c r="H12" s="74">
+      <c r="H12" s="96">
         <v>4</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="69"/>
-      <c r="B13" s="93"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="84">
+      <c r="A13" s="82"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="103">
         <v>5</v>
       </c>
-      <c r="E13" s="107" t="s">
+      <c r="E13" s="104" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="77" t="s">
-        <v>68</v>
-      </c>
-      <c r="G13" s="77">
+      <c r="F13" s="107" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="105">
         <v>12</v>
       </c>
-      <c r="H13" s="77">
+      <c r="H13" s="105">
         <v>2</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="69"/>
-      <c r="B14" s="94"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="82">
+      <c r="A14" s="82"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="97">
         <v>6</v>
       </c>
-      <c r="E14" s="105" t="s">
+      <c r="E14" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="75" t="s">
-        <v>84</v>
-      </c>
-      <c r="G14" s="75">
+      <c r="F14" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="99">
         <v>0</v>
       </c>
-      <c r="H14" s="75">
+      <c r="H14" s="99">
         <v>8</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="69"/>
-      <c r="B15" s="92">
+      <c r="A15" s="82"/>
+      <c r="B15" s="77">
         <v>4</v>
       </c>
-      <c r="C15" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="83">
+      <c r="C15" s="78" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="100">
         <v>1</v>
       </c>
-      <c r="E15" s="106" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="76" t="s">
-        <v>82</v>
-      </c>
-      <c r="G15" s="76"/>
-      <c r="H15" s="76">
+      <c r="E15" s="101" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="102" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="102"/>
+      <c r="H15" s="102">
         <v>8</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="69"/>
-      <c r="B16" s="93"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="81">
+      <c r="A16" s="82"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="94">
         <v>2</v>
       </c>
-      <c r="E16" s="104" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="74">
+      <c r="E16" s="95" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="96"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="96">
         <v>8</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="69"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="81">
+      <c r="A17" s="82"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="82"/>
+      <c r="D17" s="94">
         <v>3</v>
       </c>
-      <c r="E17" s="104" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74">
+      <c r="E17" s="95" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96">
         <v>4</v>
       </c>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="69"/>
-      <c r="B18" s="93"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="81">
+      <c r="A18" s="82"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="82"/>
+      <c r="D18" s="94">
         <v>4</v>
       </c>
-      <c r="E18" s="104" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="74">
+      <c r="E18" s="95" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="96"/>
+      <c r="G18" s="96"/>
+      <c r="H18" s="96">
         <v>4</v>
       </c>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="69"/>
-      <c r="B19" s="93"/>
-      <c r="C19" s="69"/>
-      <c r="D19" s="84">
+      <c r="A19" s="82"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="103">
         <v>5</v>
       </c>
-      <c r="E19" s="107" t="s">
+      <c r="E19" s="104" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="77" t="s">
-        <v>68</v>
-      </c>
-      <c r="G19" s="77"/>
-      <c r="H19" s="77">
+      <c r="F19" s="107" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="105"/>
+      <c r="H19" s="105">
         <v>2</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="69"/>
-      <c r="B20" s="94"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="82">
+      <c r="A20" s="82"/>
+      <c r="B20" s="86"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="97">
         <v>6</v>
       </c>
-      <c r="E20" s="105" t="s">
+      <c r="E20" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="75" t="s">
-        <v>84</v>
-      </c>
-      <c r="G20" s="75"/>
-      <c r="H20" s="75">
+      <c r="F20" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="99"/>
+      <c r="H20" s="99">
         <v>8</v>
       </c>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="69"/>
-      <c r="B21" s="92">
+      <c r="A21" s="82"/>
+      <c r="B21" s="77">
         <v>5</v>
       </c>
-      <c r="C21" s="68" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="78">
+      <c r="C21" s="108" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="79">
         <v>1</v>
       </c>
-      <c r="E21" s="100" t="s">
+      <c r="E21" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="71" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" s="71">
+      <c r="F21" s="81" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="81">
         <v>91</v>
       </c>
-      <c r="H21" s="71">
+      <c r="H21" s="81">
         <v>60</v>
       </c>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="69"/>
-      <c r="B22" s="93"/>
-      <c r="C22" s="69"/>
-      <c r="D22" s="79">
+      <c r="A22" s="82"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="83">
         <v>2</v>
       </c>
-      <c r="E22" s="101" t="s">
+      <c r="E22" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="72" t="s">
-        <v>67</v>
-      </c>
-      <c r="G22" s="72">
+      <c r="F22" s="85" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" s="85">
         <v>80</v>
       </c>
-      <c r="H22" s="72">
+      <c r="H22" s="85">
         <v>60</v>
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="69"/>
-      <c r="B23" s="93"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="79">
+      <c r="A23" s="82"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="82"/>
+      <c r="D23" s="83">
         <v>3</v>
       </c>
-      <c r="E23" s="101" t="s">
+      <c r="E23" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72">
+      <c r="F23" s="85" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="85"/>
+      <c r="H23" s="85">
         <v>10</v>
       </c>
-      <c r="I23" s="8"/>
+      <c r="I23" s="8">
+        <v>12</v>
+      </c>
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="69"/>
-      <c r="B24" s="93"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="79">
+      <c r="A24" s="82"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="83">
         <v>4</v>
       </c>
-      <c r="E24" s="101" t="s">
+      <c r="E24" s="84" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="69" t="s">
+      <c r="F24" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="G24" s="72"/>
-      <c r="H24" s="72">
+      <c r="G24" s="85"/>
+      <c r="H24" s="85">
         <v>2</v>
       </c>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="69"/>
-      <c r="B25" s="93"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="79">
+      <c r="A25" s="82"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="82"/>
+      <c r="D25" s="83">
         <v>5</v>
       </c>
-      <c r="E25" s="101" t="s">
+      <c r="E25" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="F25" s="69"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="72">
+      <c r="F25" s="82"/>
+      <c r="G25" s="85"/>
+      <c r="H25" s="85">
         <v>2</v>
       </c>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="69"/>
-      <c r="B26" s="93"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="80">
+      <c r="A26" s="82"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="82"/>
+      <c r="D26" s="88">
         <v>6</v>
       </c>
-      <c r="E26" s="101" t="s">
+      <c r="E26" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="72">
+      <c r="F26" s="85" t="s">
+        <v>97</v>
+      </c>
+      <c r="G26" s="85"/>
+      <c r="H26" s="85">
         <v>20</v>
       </c>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
     </row>
     <row r="27" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="70"/>
-      <c r="B27" s="94"/>
-      <c r="C27" s="70"/>
-      <c r="D27" s="85">
+      <c r="A27" s="87"/>
+      <c r="B27" s="86"/>
+      <c r="C27" s="87"/>
+      <c r="D27" s="106">
         <v>7</v>
       </c>
-      <c r="E27" s="102" t="s">
+      <c r="E27" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="73" t="s">
-        <v>46</v>
-      </c>
-      <c r="G27" s="73"/>
-      <c r="H27" s="73">
+      <c r="F27" s="90" t="s">
+        <v>97</v>
+      </c>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90">
         <v>10</v>
       </c>
       <c r="I27" s="8"/>
@@ -3229,23 +3227,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="A3:A27"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="B21:B27"/>
+    <mergeCell ref="C21:C27"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="B15:B20"/>
     <mergeCell ref="K5:M5"/>
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="C9:C14"/>
     <mergeCell ref="B9:B14"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B21:B27"/>
-    <mergeCell ref="C21:C27"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="A3:A27"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="G3:G5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modify 3d print design 6
</commit_message>
<xml_diff>
--- a/3d modeling/part list.xlsx
+++ b/3d modeling/part list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mokhw\Desktop\GitHub\gyroscope-drone\3d modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4CC53F-3B73-4735-BB62-EE99FC6253C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E7E8EF-CB0C-4CCC-A9CC-888279A44E6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F276262A-D9E6-428D-93CB-A151E407799A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="100">
   <si>
     <t>axis</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -360,14 +360,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>roll-ring</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pitch-ring</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[roll-ring] frame</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -393,14 +385,6 @@
   </si>
   <si>
     <t>inner Φ4, outer Φ7, width 2.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>inner Φ380, outer Φ400, thickness 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>inner Φ420, outer Φ440, thickness 10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -439,14 +423,6 @@
   </si>
   <si>
     <t>[pitch-ring] bracket-basic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[pitch-ring]  bracket-pitch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[pitch-ring]  bracket-yaw</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -482,6 +458,208 @@
   </si>
   <si>
     <t>hole Φ3.2</t>
+  </si>
+  <si>
+    <t>5hub-yaw-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5hub-yaw-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">inner </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Φ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="나눔고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">380, outer </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Φ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="나눔고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>400, thickness 10</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">roll-ring
+(inner </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Φ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="나눔고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">380, outer </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Φ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="나눔고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>400)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">inner </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Φ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="나눔고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">420, outer </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Φ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="나눔고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>440, thickness 10</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">pitch-ring
+(inner </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Φ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="나눔고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">420, outer </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Φ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="나눔고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>440)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[pitch-ring] bracket-pitch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[pitch-ring] bracket-yaw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1294,37 +1472,97 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="26" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="25" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1360,7 +1598,37 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1372,112 +1640,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="26" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="25" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="28" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2008,16 +2186,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="4"/>
@@ -2028,17 +2206,17 @@
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53" t="s">
+      <c r="C2" s="95"/>
+      <c r="D2" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
       <c r="I2" s="8"/>
       <c r="J2" s="6"/>
       <c r="K2" s="4"/>
@@ -2074,13 +2252,13 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="62">
+      <c r="B4" s="82">
         <v>1</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="85" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="11">
@@ -2090,7 +2268,7 @@
         <v>27</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="54">
+      <c r="G4" s="96">
         <v>468</v>
       </c>
       <c r="H4" s="13">
@@ -2100,9 +2278,9 @@
       <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="63"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="66"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="86"/>
       <c r="D5" s="15">
         <v>2</v>
       </c>
@@ -2110,7 +2288,7 @@
         <v>28</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="55"/>
+      <c r="G5" s="97"/>
       <c r="H5" s="16">
         <v>4</v>
       </c>
@@ -2120,9 +2298,9 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="63"/>
-      <c r="B6" s="64"/>
-      <c r="C6" s="67"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="87"/>
       <c r="D6" s="17">
         <v>3</v>
       </c>
@@ -2130,7 +2308,7 @@
         <v>29</v>
       </c>
       <c r="F6" s="18"/>
-      <c r="G6" s="56"/>
+      <c r="G6" s="98"/>
       <c r="H6" s="19">
         <v>1</v>
       </c>
@@ -2141,11 +2319,11 @@
       <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="63"/>
-      <c r="B7" s="62">
+      <c r="A7" s="83"/>
+      <c r="B7" s="82">
         <v>2</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="85" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="21">
@@ -2172,9 +2350,9 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="63"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="66"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="86"/>
       <c r="D8" s="24">
         <v>2</v>
       </c>
@@ -2197,9 +2375,9 @@
       <c r="J8" s="26"/>
     </row>
     <row r="9" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="63"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="66"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="86"/>
       <c r="D9" s="27">
         <v>3</v>
       </c>
@@ -2222,9 +2400,9 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="66"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="86"/>
       <c r="D10" s="21">
         <v>4</v>
       </c>
@@ -2245,9 +2423,9 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="63"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="66"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="86"/>
       <c r="D11" s="24">
         <v>5</v>
       </c>
@@ -2267,16 +2445,16 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="J11" s="46" t="s">
+      <c r="J11" s="88" t="s">
         <v>71</v>
       </c>
-      <c r="K11" s="47"/>
-      <c r="L11" s="48"/>
+      <c r="K11" s="89"/>
+      <c r="L11" s="90"/>
     </row>
     <row r="12" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="63"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="66"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="86"/>
       <c r="D12" s="24">
         <v>6</v>
       </c>
@@ -2294,16 +2472,16 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="J12" s="49" t="s">
+      <c r="J12" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="K12" s="50"/>
-      <c r="L12" s="51"/>
+      <c r="K12" s="92"/>
+      <c r="L12" s="93"/>
     </row>
     <row r="13" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="63"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="66"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="86"/>
       <c r="D13" s="24">
         <v>7</v>
       </c>
@@ -2324,9 +2502,9 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="63"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="66"/>
+      <c r="A14" s="83"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="86"/>
       <c r="D14" s="24">
         <v>8</v>
       </c>
@@ -2347,9 +2525,9 @@
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="63"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="66"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="86"/>
       <c r="D15" s="24">
         <v>9</v>
       </c>
@@ -2372,9 +2550,9 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="63"/>
-      <c r="B16" s="63"/>
-      <c r="C16" s="66"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="86"/>
       <c r="D16" s="27">
         <v>10</v>
       </c>
@@ -2393,9 +2571,9 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="63"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="66"/>
+      <c r="A17" s="83"/>
+      <c r="B17" s="83"/>
+      <c r="C17" s="86"/>
       <c r="D17" s="24">
         <v>11</v>
       </c>
@@ -2417,9 +2595,9 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="63"/>
-      <c r="B18" s="64"/>
-      <c r="C18" s="67"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="84"/>
+      <c r="C18" s="87"/>
       <c r="D18" s="27">
         <v>12</v>
       </c>
@@ -2439,11 +2617,11 @@
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="63"/>
-      <c r="B19" s="62">
+      <c r="A19" s="83"/>
+      <c r="B19" s="82">
         <v>3</v>
       </c>
-      <c r="C19" s="59" t="s">
+      <c r="C19" s="79" t="s">
         <v>51</v>
       </c>
       <c r="D19" s="21">
@@ -2467,9 +2645,9 @@
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="63"/>
-      <c r="B20" s="63"/>
-      <c r="C20" s="60"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="80"/>
       <c r="D20" s="27">
         <v>2</v>
       </c>
@@ -2491,9 +2669,9 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="63"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="60"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="80"/>
       <c r="D21" s="21">
         <v>3</v>
       </c>
@@ -2509,16 +2687,16 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="63"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="60"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="83"/>
+      <c r="C22" s="80"/>
       <c r="D22" s="24">
         <v>4</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="57" t="s">
+      <c r="F22" s="77" t="s">
         <v>47</v>
       </c>
       <c r="G22" s="43"/>
@@ -2529,16 +2707,16 @@
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="63"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="60"/>
+      <c r="A23" s="83"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="80"/>
       <c r="D23" s="24">
         <v>5</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="F23" s="58"/>
+      <c r="F23" s="78"/>
       <c r="G23" s="44"/>
       <c r="H23" s="25">
         <v>2</v>
@@ -2547,9 +2725,9 @@
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="63"/>
-      <c r="B24" s="63"/>
-      <c r="C24" s="60"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="80"/>
       <c r="D24" s="24">
         <v>6</v>
       </c>
@@ -2565,9 +2743,9 @@
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="64"/>
-      <c r="B25" s="64"/>
-      <c r="C25" s="61"/>
+      <c r="A25" s="84"/>
+      <c r="B25" s="84"/>
+      <c r="C25" s="81"/>
       <c r="D25" s="27">
         <v>7</v>
       </c>
@@ -2595,6 +2773,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G4:G6"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="C19:C25"/>
     <mergeCell ref="B19:B25"/>
@@ -2603,12 +2787,6 @@
     <mergeCell ref="C7:C18"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="B4:B6"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="G4:G6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2620,15 +2798,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49756507-D464-4B18-B1BA-D41ABE0D1473}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.125" customWidth="1"/>
     <col min="2" max="2" width="10.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.25" style="1" customWidth="1"/>
     <col min="5" max="5" width="23.875" style="1" customWidth="1"/>
     <col min="6" max="6" width="40.5" customWidth="1"/>
@@ -2639,20 +2817,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70" t="s">
+      <c r="C1" s="100"/>
+      <c r="D1" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="71"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="101"/>
       <c r="I1" s="8"/>
       <c r="J1" s="6"/>
       <c r="K1" s="4"/>
@@ -2660,72 +2838,72 @@
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="75" t="s">
+      <c r="E2" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="73" t="s">
+      <c r="F2" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="73" t="s">
+      <c r="G2" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="73" t="s">
+      <c r="H2" s="48" t="s">
         <v>39</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="102" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="77">
+      <c r="B3" s="105">
         <v>1</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="107" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="79">
+      <c r="D3" s="51">
         <v>1</v>
       </c>
-      <c r="E3" s="80" t="s">
+      <c r="E3" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="81"/>
-      <c r="G3" s="78">
+      <c r="F3" s="53"/>
+      <c r="G3" s="107">
         <v>468</v>
       </c>
-      <c r="H3" s="81">
+      <c r="H3" s="53">
         <v>2</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="82"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="83">
+      <c r="A4" s="103"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="54">
         <v>2</v>
       </c>
-      <c r="E4" s="84" t="s">
+      <c r="E4" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="85">
+      <c r="F4" s="56"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="56">
         <v>4</v>
       </c>
       <c r="I4" s="8"/>
@@ -2734,74 +2912,74 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="82"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="88">
+      <c r="A5" s="103"/>
+      <c r="B5" s="106"/>
+      <c r="C5" s="104"/>
+      <c r="D5" s="57">
         <v>3</v>
       </c>
-      <c r="E5" s="89" t="s">
+      <c r="E5" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="90"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="90">
+      <c r="F5" s="59"/>
+      <c r="G5" s="104"/>
+      <c r="H5" s="59">
         <v>1</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="47" t="s">
+      <c r="K5" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="L5" s="47"/>
-      <c r="M5" s="48"/>
+      <c r="L5" s="89"/>
+      <c r="M5" s="90"/>
     </row>
     <row r="6" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="82"/>
-      <c r="B6" s="77">
+      <c r="A6" s="103"/>
+      <c r="B6" s="105">
         <v>2</v>
       </c>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="107" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="91">
+      <c r="D6" s="60">
         <v>1</v>
       </c>
-      <c r="E6" s="92" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="93" t="s">
+      <c r="E6" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="93">
+      <c r="G6" s="62">
         <v>36</v>
       </c>
-      <c r="H6" s="93">
+      <c r="H6" s="62">
         <v>1</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="K6" s="50" t="s">
+      <c r="K6" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="L6" s="50"/>
-      <c r="M6" s="51"/>
+      <c r="L6" s="92"/>
+      <c r="M6" s="93"/>
     </row>
     <row r="7" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="82"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="94">
+      <c r="A7" s="103"/>
+      <c r="B7" s="92"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="63">
         <v>2</v>
       </c>
-      <c r="E7" s="95" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="96">
+      <c r="E7" s="64" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65">
         <v>4</v>
       </c>
       <c r="I7" s="8"/>
@@ -2809,20 +2987,20 @@
       <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="82"/>
-      <c r="B8" s="86"/>
-      <c r="C8" s="87"/>
-      <c r="D8" s="97">
+      <c r="A8" s="103"/>
+      <c r="B8" s="106"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="66">
         <v>3</v>
       </c>
-      <c r="E8" s="98" t="s">
+      <c r="E8" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="99" t="s">
-        <v>85</v>
-      </c>
-      <c r="G8" s="99"/>
-      <c r="H8" s="99">
+      <c r="F8" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68">
         <v>4</v>
       </c>
       <c r="I8" s="8"/>
@@ -2832,309 +3010,309 @@
       <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="82"/>
-      <c r="B9" s="77">
+      <c r="A9" s="103"/>
+      <c r="B9" s="105">
         <v>3</v>
       </c>
-      <c r="C9" s="78" t="s">
+      <c r="C9" s="108" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="69">
+        <v>1</v>
+      </c>
+      <c r="E9" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="100">
-        <v>1</v>
-      </c>
-      <c r="E9" s="101" t="s">
+      <c r="F9" s="71" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="71">
+        <v>10</v>
+      </c>
+      <c r="H9" s="71">
+        <v>8</v>
+      </c>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="103"/>
+      <c r="B10" s="92"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="63">
+        <v>2</v>
+      </c>
+      <c r="E10" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65">
+        <v>8</v>
+      </c>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="103"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="63">
+        <v>3</v>
+      </c>
+      <c r="E11" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="102" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="102">
-        <v>10</v>
-      </c>
-      <c r="H9" s="102">
-        <v>8</v>
-      </c>
-      <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="82"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="94">
-        <v>2</v>
-      </c>
-      <c r="E10" s="95" t="s">
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65">
+        <v>4</v>
+      </c>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="103"/>
+      <c r="B12" s="92"/>
+      <c r="C12" s="103"/>
+      <c r="D12" s="63">
+        <v>4</v>
+      </c>
+      <c r="E12" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="F10" s="96"/>
-      <c r="G10" s="96"/>
-      <c r="H10" s="96">
-        <v>8</v>
-      </c>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="82"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="82"/>
-      <c r="D11" s="94">
-        <v>3</v>
-      </c>
-      <c r="E11" s="95" t="s">
-        <v>81</v>
-      </c>
-      <c r="F11" s="96"/>
-      <c r="G11" s="96"/>
-      <c r="H11" s="96">
-        <v>4</v>
-      </c>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="82"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="94">
-        <v>4</v>
-      </c>
-      <c r="E12" s="95" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="96"/>
-      <c r="G12" s="96">
+      <c r="F12" s="65"/>
+      <c r="G12" s="65">
         <v>12</v>
       </c>
-      <c r="H12" s="96">
+      <c r="H12" s="65">
         <v>4</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="82"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="103">
+      <c r="A13" s="103"/>
+      <c r="B13" s="92"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="72">
         <v>5</v>
       </c>
-      <c r="E13" s="104" t="s">
+      <c r="E13" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="107" t="s">
-        <v>90</v>
-      </c>
-      <c r="G13" s="105">
+      <c r="F13" s="76" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="74">
         <v>12</v>
       </c>
-      <c r="H13" s="105">
+      <c r="H13" s="74">
         <v>2</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="82"/>
-      <c r="B14" s="86"/>
-      <c r="C14" s="87"/>
-      <c r="D14" s="97">
+      <c r="A14" s="103"/>
+      <c r="B14" s="106"/>
+      <c r="C14" s="104"/>
+      <c r="D14" s="66">
         <v>6</v>
       </c>
-      <c r="E14" s="98" t="s">
+      <c r="E14" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="99" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="99">
+      <c r="F14" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" s="68">
         <v>0</v>
       </c>
-      <c r="H14" s="99">
+      <c r="H14" s="68">
         <v>8</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="82"/>
-      <c r="B15" s="77">
+      <c r="A15" s="103"/>
+      <c r="B15" s="105">
         <v>4</v>
       </c>
-      <c r="C15" s="78" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="100">
+      <c r="C15" s="108" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="69">
         <v>1</v>
       </c>
-      <c r="E15" s="101" t="s">
-        <v>91</v>
-      </c>
-      <c r="F15" s="102" t="s">
+      <c r="E15" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="102"/>
-      <c r="H15" s="102">
+      <c r="F15" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="71"/>
+      <c r="H15" s="71">
         <v>8</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="82"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="94">
+      <c r="A16" s="103"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="103"/>
+      <c r="D16" s="63">
         <v>2</v>
       </c>
-      <c r="E16" s="95" t="s">
-        <v>92</v>
-      </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="96">
+      <c r="E16" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65">
         <v>8</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="82"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="94">
+      <c r="A17" s="103"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="103"/>
+      <c r="D17" s="63">
         <v>3</v>
       </c>
-      <c r="E17" s="95" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" s="96"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96">
+      <c r="E17" s="64" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65">
         <v>4</v>
       </c>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="82"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="94">
+      <c r="A18" s="103"/>
+      <c r="B18" s="92"/>
+      <c r="C18" s="103"/>
+      <c r="D18" s="63">
         <v>4</v>
       </c>
-      <c r="E18" s="95" t="s">
-        <v>94</v>
-      </c>
-      <c r="F18" s="96"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="96">
+      <c r="E18" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65">
         <v>4</v>
       </c>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="82"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="103">
+      <c r="A19" s="103"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="103"/>
+      <c r="D19" s="72">
         <v>5</v>
       </c>
-      <c r="E19" s="104" t="s">
+      <c r="E19" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="107" t="s">
-        <v>90</v>
-      </c>
-      <c r="G19" s="105"/>
-      <c r="H19" s="105">
+      <c r="F19" s="76" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="74"/>
+      <c r="H19" s="74">
         <v>2</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="82"/>
-      <c r="B20" s="86"/>
-      <c r="C20" s="87"/>
-      <c r="D20" s="97">
+      <c r="A20" s="103"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="104"/>
+      <c r="D20" s="66">
         <v>6</v>
       </c>
-      <c r="E20" s="98" t="s">
+      <c r="E20" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="99" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" s="99"/>
-      <c r="H20" s="99">
+      <c r="F20" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="G20" s="68"/>
+      <c r="H20" s="68">
         <v>8</v>
       </c>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="82"/>
-      <c r="B21" s="77">
+      <c r="A21" s="103"/>
+      <c r="B21" s="105">
         <v>5</v>
       </c>
       <c r="C21" s="108" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="79">
+        <v>89</v>
+      </c>
+      <c r="D21" s="51">
         <v>1</v>
       </c>
-      <c r="E21" s="80" t="s">
+      <c r="E21" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="81" t="s">
-        <v>88</v>
-      </c>
-      <c r="G21" s="81">
+      <c r="F21" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="53">
         <v>91</v>
       </c>
-      <c r="H21" s="81">
+      <c r="H21" s="53">
         <v>60</v>
       </c>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="82"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="82"/>
-      <c r="D22" s="83">
+      <c r="A22" s="103"/>
+      <c r="B22" s="92"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="54">
         <v>2</v>
       </c>
-      <c r="E22" s="84" t="s">
+      <c r="E22" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="85" t="s">
-        <v>89</v>
-      </c>
-      <c r="G22" s="85">
+      <c r="F22" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" s="56">
         <v>80</v>
       </c>
-      <c r="H22" s="85">
+      <c r="H22" s="56">
         <v>60</v>
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="82"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="82"/>
-      <c r="D23" s="83">
+      <c r="A23" s="103"/>
+      <c r="B23" s="92"/>
+      <c r="C23" s="103"/>
+      <c r="D23" s="54">
         <v>3</v>
       </c>
-      <c r="E23" s="84" t="s">
+      <c r="E23" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="G23" s="85"/>
-      <c r="H23" s="85">
+      <c r="F23" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56">
         <v>10</v>
       </c>
       <c r="I23" s="8">
@@ -3143,78 +3321,78 @@
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="82"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="82"/>
-      <c r="D24" s="83">
+      <c r="A24" s="103"/>
+      <c r="B24" s="92"/>
+      <c r="C24" s="103"/>
+      <c r="D24" s="54">
         <v>4</v>
       </c>
-      <c r="E24" s="84" t="s">
-        <v>63</v>
-      </c>
-      <c r="F24" s="82" t="s">
+      <c r="E24" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="G24" s="85"/>
-      <c r="H24" s="85">
+      <c r="G24" s="56"/>
+      <c r="H24" s="56">
         <v>2</v>
       </c>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="82"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="82"/>
-      <c r="D25" s="83">
+      <c r="A25" s="103"/>
+      <c r="B25" s="92"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="54">
         <v>5</v>
       </c>
-      <c r="E25" s="84" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" s="82"/>
-      <c r="G25" s="85"/>
-      <c r="H25" s="85">
+      <c r="E25" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="103"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56">
         <v>2</v>
       </c>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="82"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="82"/>
-      <c r="D26" s="88">
+      <c r="A26" s="103"/>
+      <c r="B26" s="92"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="57">
         <v>6</v>
       </c>
-      <c r="E26" s="84" t="s">
+      <c r="E26" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="85" t="s">
-        <v>97</v>
-      </c>
-      <c r="G26" s="85"/>
-      <c r="H26" s="85">
+      <c r="F26" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56">
         <v>20</v>
       </c>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
     </row>
     <row r="27" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="87"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="106">
+      <c r="A27" s="104"/>
+      <c r="B27" s="106"/>
+      <c r="C27" s="104"/>
+      <c r="D27" s="75">
         <v>7</v>
       </c>
-      <c r="E27" s="89" t="s">
+      <c r="E27" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="90" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" s="90"/>
-      <c r="H27" s="90">
+      <c r="F27" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59">
         <v>10</v>
       </c>
       <c r="I27" s="8"/>
@@ -3227,6 +3405,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B6:B8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="A3:A27"/>
@@ -3238,12 +3422,6 @@
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="C15:C20"/>
     <mergeCell ref="B15:B20"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="B6:B8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modify 3d print design 7
</commit_message>
<xml_diff>
--- a/3d modeling/part list.xlsx
+++ b/3d modeling/part list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mokhw\Desktop\GitHub\gyroscope-quadcopter\3d modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF74A3F-5FD7-4A11-9E4B-5B348F64EB30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8C473A-3DE0-4624-A8E5-8993521CF2C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3375" yWindow="1695" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{F276262A-D9E6-428D-93CB-A151E407799A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F276262A-D9E6-428D-93CB-A151E407799A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
   <si>
     <t>axis</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -659,6 +659,70 @@
   </si>
   <si>
     <t>[pitch-ring] bracket-yaw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>브라켓 홀 3.2로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>베어링 폭 2.6으로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bearing width 2.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">hole </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Φ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="나눔고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">3.2, bearing width 2.6 </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">hole </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="161"/>
+      </rPr>
+      <t>Φ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="나눔고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>3.2, bearing width 2.6</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1565,39 +1629,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1631,35 +1662,68 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2186,16 +2250,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="4"/>
@@ -2206,17 +2270,17 @@
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84" t="s">
+      <c r="C2" s="95"/>
+      <c r="D2" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
       <c r="I2" s="8"/>
       <c r="J2" s="6"/>
       <c r="K2" s="4"/>
@@ -2252,13 +2316,13 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="93">
+      <c r="B4" s="82">
         <v>1</v>
       </c>
-      <c r="C4" s="96" t="s">
+      <c r="C4" s="85" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="11">
@@ -2268,7 +2332,7 @@
         <v>27</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="85">
+      <c r="G4" s="96">
         <v>468</v>
       </c>
       <c r="H4" s="13">
@@ -2278,9 +2342,9 @@
       <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="94"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="97"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="86"/>
       <c r="D5" s="15">
         <v>2</v>
       </c>
@@ -2288,7 +2352,7 @@
         <v>28</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="86"/>
+      <c r="G5" s="97"/>
       <c r="H5" s="16">
         <v>4</v>
       </c>
@@ -2298,9 +2362,9 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="94"/>
-      <c r="B6" s="95"/>
-      <c r="C6" s="98"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="87"/>
       <c r="D6" s="17">
         <v>3</v>
       </c>
@@ -2308,7 +2372,7 @@
         <v>29</v>
       </c>
       <c r="F6" s="18"/>
-      <c r="G6" s="87"/>
+      <c r="G6" s="98"/>
       <c r="H6" s="19">
         <v>1</v>
       </c>
@@ -2319,11 +2383,11 @@
       <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="94"/>
-      <c r="B7" s="93">
+      <c r="A7" s="83"/>
+      <c r="B7" s="82">
         <v>2</v>
       </c>
-      <c r="C7" s="96" t="s">
+      <c r="C7" s="85" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="21">
@@ -2350,9 +2414,9 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="94"/>
-      <c r="B8" s="94"/>
-      <c r="C8" s="97"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="86"/>
       <c r="D8" s="24">
         <v>2</v>
       </c>
@@ -2375,9 +2439,9 @@
       <c r="J8" s="26"/>
     </row>
     <row r="9" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="94"/>
-      <c r="B9" s="94"/>
-      <c r="C9" s="97"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="86"/>
       <c r="D9" s="27">
         <v>3</v>
       </c>
@@ -2400,9 +2464,9 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="94"/>
-      <c r="B10" s="94"/>
-      <c r="C10" s="97"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="86"/>
       <c r="D10" s="21">
         <v>4</v>
       </c>
@@ -2423,9 +2487,9 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="94"/>
-      <c r="B11" s="94"/>
-      <c r="C11" s="97"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="86"/>
       <c r="D11" s="24">
         <v>5</v>
       </c>
@@ -2445,16 +2509,16 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="J11" s="77" t="s">
+      <c r="J11" s="88" t="s">
         <v>71</v>
       </c>
-      <c r="K11" s="78"/>
-      <c r="L11" s="79"/>
+      <c r="K11" s="89"/>
+      <c r="L11" s="90"/>
     </row>
     <row r="12" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="94"/>
-      <c r="B12" s="94"/>
-      <c r="C12" s="97"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="86"/>
       <c r="D12" s="24">
         <v>6</v>
       </c>
@@ -2472,16 +2536,16 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="J12" s="80" t="s">
+      <c r="J12" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="K12" s="81"/>
-      <c r="L12" s="82"/>
+      <c r="K12" s="92"/>
+      <c r="L12" s="93"/>
     </row>
     <row r="13" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="94"/>
-      <c r="B13" s="94"/>
-      <c r="C13" s="97"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="86"/>
       <c r="D13" s="24">
         <v>7</v>
       </c>
@@ -2502,9 +2566,9 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="94"/>
-      <c r="B14" s="94"/>
-      <c r="C14" s="97"/>
+      <c r="A14" s="83"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="86"/>
       <c r="D14" s="24">
         <v>8</v>
       </c>
@@ -2525,9 +2589,9 @@
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="94"/>
-      <c r="B15" s="94"/>
-      <c r="C15" s="97"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="86"/>
       <c r="D15" s="24">
         <v>9</v>
       </c>
@@ -2550,9 +2614,9 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="94"/>
-      <c r="B16" s="94"/>
-      <c r="C16" s="97"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="86"/>
       <c r="D16" s="27">
         <v>10</v>
       </c>
@@ -2571,9 +2635,9 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="94"/>
-      <c r="B17" s="94"/>
-      <c r="C17" s="97"/>
+      <c r="A17" s="83"/>
+      <c r="B17" s="83"/>
+      <c r="C17" s="86"/>
       <c r="D17" s="24">
         <v>11</v>
       </c>
@@ -2595,9 +2659,9 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="94"/>
-      <c r="B18" s="95"/>
-      <c r="C18" s="98"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="84"/>
+      <c r="C18" s="87"/>
       <c r="D18" s="27">
         <v>12</v>
       </c>
@@ -2617,11 +2681,11 @@
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="94"/>
-      <c r="B19" s="93">
+      <c r="A19" s="83"/>
+      <c r="B19" s="82">
         <v>3</v>
       </c>
-      <c r="C19" s="90" t="s">
+      <c r="C19" s="79" t="s">
         <v>51</v>
       </c>
       <c r="D19" s="21">
@@ -2645,9 +2709,9 @@
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="94"/>
-      <c r="B20" s="94"/>
-      <c r="C20" s="91"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="80"/>
       <c r="D20" s="27">
         <v>2</v>
       </c>
@@ -2669,9 +2733,9 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="94"/>
-      <c r="B21" s="94"/>
-      <c r="C21" s="91"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="80"/>
       <c r="D21" s="21">
         <v>3</v>
       </c>
@@ -2687,16 +2751,16 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="94"/>
-      <c r="B22" s="94"/>
-      <c r="C22" s="91"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="83"/>
+      <c r="C22" s="80"/>
       <c r="D22" s="24">
         <v>4</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="88" t="s">
+      <c r="F22" s="77" t="s">
         <v>47</v>
       </c>
       <c r="G22" s="43"/>
@@ -2707,16 +2771,16 @@
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="94"/>
-      <c r="B23" s="94"/>
-      <c r="C23" s="91"/>
+      <c r="A23" s="83"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="80"/>
       <c r="D23" s="24">
         <v>5</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="F23" s="89"/>
+      <c r="F23" s="78"/>
       <c r="G23" s="44"/>
       <c r="H23" s="25">
         <v>2</v>
@@ -2725,9 +2789,9 @@
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="94"/>
-      <c r="B24" s="94"/>
-      <c r="C24" s="91"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="80"/>
       <c r="D24" s="24">
         <v>6</v>
       </c>
@@ -2743,9 +2807,9 @@
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="95"/>
-      <c r="B25" s="95"/>
-      <c r="C25" s="92"/>
+      <c r="A25" s="84"/>
+      <c r="B25" s="84"/>
+      <c r="C25" s="81"/>
       <c r="D25" s="27">
         <v>7</v>
       </c>
@@ -2773,6 +2837,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G4:G6"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="C19:C25"/>
     <mergeCell ref="B19:B25"/>
@@ -2781,12 +2851,6 @@
     <mergeCell ref="C7:C18"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="B4:B6"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="G4:G6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2798,8 +2862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49756507-D464-4B18-B1BA-D41ABE0D1473}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2820,17 +2884,17 @@
       <c r="A1" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="105" t="s">
+      <c r="B1" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106" t="s">
+      <c r="C1" s="100"/>
+      <c r="D1" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="107"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="101"/>
       <c r="I1" s="8"/>
       <c r="J1" s="6"/>
       <c r="K1" s="4"/>
@@ -2866,13 +2930,13 @@
       <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="102" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="102">
+      <c r="B3" s="105">
         <v>1</v>
       </c>
-      <c r="C3" s="104" t="s">
+      <c r="C3" s="107" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="51">
@@ -2882,7 +2946,7 @@
         <v>27</v>
       </c>
       <c r="F3" s="53"/>
-      <c r="G3" s="104">
+      <c r="G3" s="107">
         <v>468</v>
       </c>
       <c r="H3" s="53">
@@ -2892,9 +2956,9 @@
       <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="100"/>
-      <c r="B4" s="81"/>
-      <c r="C4" s="100"/>
+      <c r="A4" s="103"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="103"/>
       <c r="D4" s="54">
         <v>2</v>
       </c>
@@ -2902,7 +2966,7 @@
         <v>28</v>
       </c>
       <c r="F4" s="56"/>
-      <c r="G4" s="100"/>
+      <c r="G4" s="103"/>
       <c r="H4" s="56">
         <v>4</v>
       </c>
@@ -2912,9 +2976,9 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="100"/>
-      <c r="B5" s="103"/>
-      <c r="C5" s="101"/>
+      <c r="A5" s="103"/>
+      <c r="B5" s="106"/>
+      <c r="C5" s="104"/>
       <c r="D5" s="57">
         <v>3</v>
       </c>
@@ -2922,24 +2986,24 @@
         <v>29</v>
       </c>
       <c r="F5" s="59"/>
-      <c r="G5" s="101"/>
+      <c r="G5" s="104"/>
       <c r="H5" s="59">
         <v>1</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="78" t="s">
+      <c r="K5" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="L5" s="78"/>
-      <c r="M5" s="79"/>
+      <c r="L5" s="89"/>
+      <c r="M5" s="90"/>
     </row>
     <row r="6" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="100"/>
-      <c r="B6" s="102">
+      <c r="A6" s="103"/>
+      <c r="B6" s="105">
         <v>2</v>
       </c>
-      <c r="C6" s="104" t="s">
+      <c r="C6" s="107" t="s">
         <v>74</v>
       </c>
       <c r="D6" s="60">
@@ -2961,16 +3025,16 @@
       <c r="J6" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="K6" s="81" t="s">
+      <c r="K6" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="L6" s="81"/>
-      <c r="M6" s="82"/>
+      <c r="L6" s="92"/>
+      <c r="M6" s="93"/>
     </row>
     <row r="7" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="100"/>
-      <c r="B7" s="81"/>
-      <c r="C7" s="100"/>
+      <c r="A7" s="103"/>
+      <c r="B7" s="92"/>
+      <c r="C7" s="103"/>
       <c r="D7" s="63">
         <v>2</v>
       </c>
@@ -2987,9 +3051,9 @@
       <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="100"/>
-      <c r="B8" s="103"/>
-      <c r="C8" s="101"/>
+      <c r="A8" s="103"/>
+      <c r="B8" s="106"/>
+      <c r="C8" s="104"/>
       <c r="D8" s="66">
         <v>3</v>
       </c>
@@ -3010,11 +3074,11 @@
       <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="100"/>
-      <c r="B9" s="102">
+      <c r="A9" s="103"/>
+      <c r="B9" s="105">
         <v>3</v>
       </c>
-      <c r="C9" s="99" t="s">
+      <c r="C9" s="108" t="s">
         <v>95</v>
       </c>
       <c r="D9" s="69">
@@ -3035,9 +3099,9 @@
       <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="100"/>
-      <c r="B10" s="81"/>
-      <c r="C10" s="100"/>
+      <c r="A10" s="103"/>
+      <c r="B10" s="92"/>
+      <c r="C10" s="103"/>
       <c r="D10" s="63">
         <v>2</v>
       </c>
@@ -3050,35 +3114,45 @@
         <v>8</v>
       </c>
       <c r="I10" s="8"/>
+      <c r="J10" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="100"/>
-      <c r="B11" s="81"/>
-      <c r="C11" s="100"/>
+      <c r="A11" s="103"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="103"/>
       <c r="D11" s="63">
         <v>3</v>
       </c>
       <c r="E11" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="65"/>
+      <c r="F11" s="65" t="s">
+        <v>103</v>
+      </c>
       <c r="G11" s="65"/>
       <c r="H11" s="65">
         <v>4</v>
       </c>
       <c r="I11" s="8"/>
+      <c r="J11" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="100"/>
-      <c r="B12" s="81"/>
-      <c r="C12" s="100"/>
+      <c r="A12" s="103"/>
+      <c r="B12" s="92"/>
+      <c r="C12" s="103"/>
       <c r="D12" s="63">
         <v>4</v>
       </c>
       <c r="E12" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="65"/>
+      <c r="F12" s="65" t="s">
+        <v>104</v>
+      </c>
       <c r="G12" s="65">
         <v>12</v>
       </c>
@@ -3086,12 +3160,14 @@
         <v>4</v>
       </c>
       <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="J12" s="8" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="100"/>
-      <c r="B13" s="81"/>
-      <c r="C13" s="100"/>
+      <c r="A13" s="103"/>
+      <c r="B13" s="92"/>
+      <c r="C13" s="103"/>
       <c r="D13" s="72">
         <v>5</v>
       </c>
@@ -3111,9 +3187,9 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="100"/>
-      <c r="B14" s="103"/>
-      <c r="C14" s="101"/>
+      <c r="A14" s="103"/>
+      <c r="B14" s="106"/>
+      <c r="C14" s="104"/>
       <c r="D14" s="66">
         <v>6</v>
       </c>
@@ -3133,11 +3209,11 @@
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="100"/>
-      <c r="B15" s="102">
+      <c r="A15" s="103"/>
+      <c r="B15" s="105">
         <v>4</v>
       </c>
-      <c r="C15" s="99" t="s">
+      <c r="C15" s="108" t="s">
         <v>97</v>
       </c>
       <c r="D15" s="69">
@@ -3157,9 +3233,9 @@
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="100"/>
-      <c r="B16" s="81"/>
-      <c r="C16" s="100"/>
+      <c r="A16" s="103"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="103"/>
       <c r="D16" s="63">
         <v>2</v>
       </c>
@@ -3175,16 +3251,18 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="100"/>
-      <c r="B17" s="81"/>
-      <c r="C17" s="100"/>
+      <c r="A17" s="103"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="103"/>
       <c r="D17" s="63">
         <v>3</v>
       </c>
       <c r="E17" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="F17" s="65"/>
+      <c r="F17" s="65" t="s">
+        <v>103</v>
+      </c>
       <c r="G17" s="65"/>
       <c r="H17" s="65">
         <v>4</v>
@@ -3193,16 +3271,18 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="100"/>
-      <c r="B18" s="81"/>
-      <c r="C18" s="100"/>
+      <c r="A18" s="103"/>
+      <c r="B18" s="92"/>
+      <c r="C18" s="103"/>
       <c r="D18" s="63">
         <v>4</v>
       </c>
       <c r="E18" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="F18" s="65"/>
+      <c r="F18" s="65" t="s">
+        <v>103</v>
+      </c>
       <c r="G18" s="65"/>
       <c r="H18" s="65">
         <v>4</v>
@@ -3211,9 +3291,9 @@
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="100"/>
-      <c r="B19" s="81"/>
-      <c r="C19" s="100"/>
+      <c r="A19" s="103"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="103"/>
       <c r="D19" s="72">
         <v>5</v>
       </c>
@@ -3231,9 +3311,9 @@
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="100"/>
-      <c r="B20" s="103"/>
-      <c r="C20" s="101"/>
+      <c r="A20" s="103"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="104"/>
       <c r="D20" s="66">
         <v>6</v>
       </c>
@@ -3251,11 +3331,11 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="100"/>
-      <c r="B21" s="102">
+      <c r="A21" s="103"/>
+      <c r="B21" s="105">
         <v>5</v>
       </c>
-      <c r="C21" s="99" t="s">
+      <c r="C21" s="108" t="s">
         <v>89</v>
       </c>
       <c r="D21" s="51">
@@ -3277,9 +3357,9 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="100"/>
-      <c r="B22" s="81"/>
-      <c r="C22" s="100"/>
+      <c r="A22" s="103"/>
+      <c r="B22" s="92"/>
+      <c r="C22" s="103"/>
       <c r="D22" s="54">
         <v>2</v>
       </c>
@@ -3299,9 +3379,9 @@
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="100"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="100"/>
+      <c r="A23" s="103"/>
+      <c r="B23" s="92"/>
+      <c r="C23" s="103"/>
       <c r="D23" s="54">
         <v>3</v>
       </c>
@@ -3321,16 +3401,16 @@
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="100"/>
-      <c r="B24" s="81"/>
-      <c r="C24" s="100"/>
+      <c r="A24" s="103"/>
+      <c r="B24" s="92"/>
+      <c r="C24" s="103"/>
       <c r="D24" s="54">
         <v>4</v>
       </c>
       <c r="E24" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="F24" s="100" t="s">
+      <c r="F24" s="103" t="s">
         <v>47</v>
       </c>
       <c r="G24" s="56"/>
@@ -3341,16 +3421,16 @@
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="100"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="100"/>
+      <c r="A25" s="103"/>
+      <c r="B25" s="92"/>
+      <c r="C25" s="103"/>
       <c r="D25" s="54">
         <v>5</v>
       </c>
       <c r="E25" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="F25" s="100"/>
+      <c r="F25" s="103"/>
       <c r="G25" s="56"/>
       <c r="H25" s="56">
         <v>2</v>
@@ -3359,9 +3439,9 @@
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="100"/>
-      <c r="B26" s="81"/>
-      <c r="C26" s="100"/>
+      <c r="A26" s="103"/>
+      <c r="B26" s="92"/>
+      <c r="C26" s="103"/>
       <c r="D26" s="57">
         <v>6</v>
       </c>
@@ -3369,7 +3449,7 @@
         <v>55</v>
       </c>
       <c r="F26" s="56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G26" s="56"/>
       <c r="H26" s="56">
@@ -3379,9 +3459,9 @@
       <c r="J26" s="8"/>
     </row>
     <row r="27" spans="1:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="101"/>
-      <c r="B27" s="103"/>
-      <c r="C27" s="101"/>
+      <c r="A27" s="104"/>
+      <c r="B27" s="106"/>
+      <c r="C27" s="104"/>
       <c r="D27" s="75">
         <v>7</v>
       </c>
@@ -3405,6 +3485,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B6:B8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="A3:A27"/>
@@ -3416,12 +3502,6 @@
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="C15:C20"/>
     <mergeCell ref="B15:B20"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="B6:B8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>